<commit_message>
Rachelle wanted these data sets updated
</commit_message>
<xml_diff>
--- a/Data/FuelEfficiency.xlsx
+++ b/Data/FuelEfficiency.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55a6387db2d930ac/Documents/BYUI/Lesson Presentations/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA34CF82-2F5D-4523-9A6B-5FE6116B9C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{EA34CF82-2F5D-4523-9A6B-5FE6116B9C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0E12648-2883-4292-8B13-538B5A83F9A3}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="19452" windowHeight="10908"/>
+    <workbookView xWindow="1548" yWindow="588" windowWidth="19452" windowHeight="10908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fuel-efficiency" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="101">
   <si>
     <t>Model</t>
   </si>
@@ -178,9 +190,6 @@
     <t>ES_330</t>
   </si>
   <si>
-    <t>Prius</t>
-  </si>
-  <si>
     <t>S40_TS</t>
   </si>
   <si>
@@ -194,9 +203,6 @@
   </si>
   <si>
     <t>Jetta_GLI</t>
-  </si>
-  <si>
-    <t>Viper</t>
   </si>
   <si>
     <t>Cooper</t>
@@ -334,7 +340,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1169,11 +1175,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,12 +1210,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>1.8</v>
@@ -2343,57 +2349,57 @@
         <v>52</v>
       </c>
       <c r="B41">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D41">
-        <v>20295</v>
+        <v>26990</v>
       </c>
       <c r="E41">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F41">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="G41">
-        <v>2890</v>
+        <v>3126</v>
       </c>
       <c r="H41" t="s">
         <v>8</v>
       </c>
       <c r="I41" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>39860</v>
+      </c>
+      <c r="E42">
+        <v>19</v>
+      </c>
+      <c r="F42">
+        <v>28</v>
+      </c>
+      <c r="G42">
+        <v>3470</v>
+      </c>
+      <c r="H42" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" t="s">
         <v>53</v>
-      </c>
-      <c r="B42">
-        <v>2.5</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42">
-        <v>26990</v>
-      </c>
-      <c r="E42">
-        <v>22</v>
-      </c>
-      <c r="F42">
-        <v>31</v>
-      </c>
-      <c r="G42">
-        <v>3126</v>
-      </c>
-      <c r="H42" t="s">
-        <v>8</v>
-      </c>
-      <c r="I42" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2401,28 +2407,28 @@
         <v>55</v>
       </c>
       <c r="B43">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="C43">
         <v>4</v>
       </c>
       <c r="D43">
-        <v>39860</v>
+        <v>26490</v>
       </c>
       <c r="E43">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F43">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G43">
-        <v>3470</v>
+        <v>3318</v>
       </c>
       <c r="H43" t="s">
         <v>8</v>
       </c>
       <c r="I43" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2430,28 +2436,28 @@
         <v>56</v>
       </c>
       <c r="B44">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D44">
-        <v>26490</v>
+        <v>23210</v>
       </c>
       <c r="E44">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F44">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G44">
-        <v>3318</v>
+        <v>3179</v>
       </c>
       <c r="H44" t="s">
         <v>8</v>
       </c>
       <c r="I44" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -2459,28 +2465,28 @@
         <v>57</v>
       </c>
       <c r="B45">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>23210</v>
+        <v>19899</v>
       </c>
       <c r="E45">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F45">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G45">
-        <v>3179</v>
+        <v>2678</v>
       </c>
       <c r="H45" t="s">
         <v>8</v>
       </c>
       <c r="I45" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -2488,25 +2494,25 @@
         <v>58</v>
       </c>
       <c r="B46">
-        <v>8.3000000000000007</v>
+        <v>2.4</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D46">
-        <v>81090</v>
+        <v>18330</v>
       </c>
       <c r="E46">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F46">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G46">
-        <v>3410</v>
+        <v>3908</v>
       </c>
       <c r="H46" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="I46" t="s">
         <v>22</v>
@@ -2514,60 +2520,60 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47">
+        <v>3.4</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>21475</v>
+      </c>
+      <c r="E47">
+        <v>19</v>
+      </c>
+      <c r="F47">
+        <v>26</v>
+      </c>
+      <c r="G47">
+        <v>3699</v>
+      </c>
+      <c r="H47" t="s">
         <v>59</v>
       </c>
-      <c r="B47">
-        <v>1.6</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-      <c r="D47">
-        <v>19899</v>
-      </c>
-      <c r="E47">
-        <v>24</v>
-      </c>
-      <c r="F47">
-        <v>33</v>
-      </c>
-      <c r="G47">
-        <v>2678</v>
-      </c>
-      <c r="H47" t="s">
-        <v>8</v>
-      </c>
       <c r="I47" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B48">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48">
-        <v>18330</v>
+        <v>22085</v>
       </c>
       <c r="E48">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F48">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G48">
-        <v>3908</v>
+        <v>4802</v>
       </c>
       <c r="H48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I48" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -2575,28 +2581,28 @@
         <v>62</v>
       </c>
       <c r="B49">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>6</v>
       </c>
       <c r="D49">
-        <v>21475</v>
+        <v>23490</v>
       </c>
       <c r="E49">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F49">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G49">
-        <v>3699</v>
+        <v>3772</v>
       </c>
       <c r="H49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I49" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2604,28 +2610,28 @@
         <v>63</v>
       </c>
       <c r="B50">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C50">
         <v>6</v>
       </c>
       <c r="D50">
-        <v>22085</v>
+        <v>23335</v>
       </c>
       <c r="E50">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F50">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G50">
-        <v>4802</v>
+        <v>3803</v>
       </c>
       <c r="H50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I50" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2633,28 +2639,28 @@
         <v>64</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="C51">
         <v>6</v>
       </c>
       <c r="D51">
-        <v>23490</v>
+        <v>26390</v>
       </c>
       <c r="E51">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F51">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G51">
-        <v>3772</v>
+        <v>4275</v>
       </c>
       <c r="H51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I51" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2662,25 +2668,25 @@
         <v>65</v>
       </c>
       <c r="B52">
-        <v>3.4</v>
+        <v>4.3</v>
       </c>
       <c r="C52">
         <v>6</v>
       </c>
       <c r="D52">
-        <v>23335</v>
+        <v>25230</v>
       </c>
       <c r="E52">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F52">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G52">
-        <v>3803</v>
+        <v>4309</v>
       </c>
       <c r="H52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I52" t="s">
         <v>22</v>
@@ -2691,28 +2697,28 @@
         <v>66</v>
       </c>
       <c r="B53">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="C53">
         <v>6</v>
       </c>
       <c r="D53">
-        <v>26390</v>
+        <v>26990</v>
       </c>
       <c r="E53">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F53">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G53">
-        <v>4275</v>
+        <v>4365</v>
       </c>
       <c r="H53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I53" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2720,28 +2726,28 @@
         <v>67</v>
       </c>
       <c r="B54">
-        <v>4.3</v>
+        <v>3.3</v>
       </c>
       <c r="C54">
         <v>6</v>
       </c>
       <c r="D54">
-        <v>25230</v>
+        <v>24480</v>
       </c>
       <c r="E54">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F54">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G54">
-        <v>4309</v>
+        <v>4120</v>
       </c>
       <c r="H54" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I54" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2749,25 +2755,25 @@
         <v>68</v>
       </c>
       <c r="B55">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D55">
-        <v>26990</v>
+        <v>21520</v>
       </c>
       <c r="E55">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F55">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G55">
-        <v>4365</v>
+        <v>3400</v>
       </c>
       <c r="H55" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="I55" t="s">
         <v>12</v>
@@ -2775,57 +2781,57 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56">
+        <v>1.9</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>25700</v>
+      </c>
+      <c r="E56">
+        <v>22</v>
+      </c>
+      <c r="F56">
+        <v>29</v>
+      </c>
+      <c r="G56">
+        <v>2822</v>
+      </c>
+      <c r="H56" t="s">
         <v>69</v>
       </c>
-      <c r="B56">
-        <v>3.3</v>
-      </c>
-      <c r="C56">
-        <v>6</v>
-      </c>
-      <c r="D56">
-        <v>24480</v>
-      </c>
-      <c r="E56">
-        <v>19</v>
-      </c>
-      <c r="F56">
-        <v>27</v>
-      </c>
-      <c r="G56">
-        <v>4120</v>
-      </c>
-      <c r="H56" t="s">
-        <v>61</v>
-      </c>
       <c r="I56" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B57">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="C57">
         <v>4</v>
       </c>
       <c r="D57">
-        <v>21520</v>
+        <v>14480</v>
       </c>
       <c r="E57">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F57">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G57">
-        <v>3400</v>
+        <v>2469</v>
       </c>
       <c r="H57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I57" t="s">
         <v>12</v>
@@ -2836,28 +2842,28 @@
         <v>72</v>
       </c>
       <c r="B58">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="C58">
         <v>4</v>
       </c>
       <c r="D58">
-        <v>25700</v>
+        <v>16605</v>
       </c>
       <c r="E58">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F58">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G58">
-        <v>2822</v>
+        <v>2700</v>
       </c>
       <c r="H58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I58" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2865,25 +2871,25 @@
         <v>73</v>
       </c>
       <c r="B59">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="C59">
         <v>4</v>
       </c>
       <c r="D59">
-        <v>14480</v>
+        <v>15470</v>
       </c>
       <c r="E59">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F59">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G59">
-        <v>2469</v>
+        <v>2756</v>
       </c>
       <c r="H59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I59" t="s">
         <v>12</v>
@@ -2894,25 +2900,25 @@
         <v>74</v>
       </c>
       <c r="B60">
-        <v>1.8</v>
+        <v>4.2</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D60">
-        <v>16605</v>
+        <v>38645</v>
       </c>
       <c r="E60">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F60">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G60">
-        <v>2700</v>
+        <v>4628</v>
       </c>
       <c r="H60" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I60" t="s">
         <v>22</v>
@@ -2920,28 +2926,28 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61">
+        <v>3.5</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>36050</v>
+      </c>
+      <c r="E61">
+        <v>16</v>
+      </c>
+      <c r="F61">
+        <v>22</v>
+      </c>
+      <c r="G61">
+        <v>4215</v>
+      </c>
+      <c r="H61" t="s">
         <v>75</v>
-      </c>
-      <c r="B61">
-        <v>1.8</v>
-      </c>
-      <c r="C61">
-        <v>4</v>
-      </c>
-      <c r="D61">
-        <v>15470</v>
-      </c>
-      <c r="E61">
-        <v>27</v>
-      </c>
-      <c r="F61">
-        <v>32</v>
-      </c>
-      <c r="G61">
-        <v>2756</v>
-      </c>
-      <c r="H61" t="s">
-        <v>71</v>
       </c>
       <c r="I61" t="s">
         <v>12</v>
@@ -2949,28 +2955,28 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B62">
-        <v>4.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D62">
-        <v>38645</v>
+        <v>38335</v>
       </c>
       <c r="E62">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F62">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G62">
-        <v>4628</v>
+        <v>4523</v>
       </c>
       <c r="H62" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I62" t="s">
         <v>22</v>
@@ -2981,28 +2987,28 @@
         <v>78</v>
       </c>
       <c r="B63">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="C63">
         <v>6</v>
       </c>
       <c r="D63">
-        <v>36050</v>
+        <v>35900</v>
       </c>
       <c r="E63">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F63">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G63">
-        <v>4215</v>
+        <v>5086</v>
       </c>
       <c r="H63" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I63" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -3010,28 +3016,28 @@
         <v>79</v>
       </c>
       <c r="B64">
-        <v>4.5999999999999996</v>
+        <v>2.9</v>
       </c>
       <c r="C64">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D64">
-        <v>38335</v>
+        <v>40695</v>
       </c>
       <c r="E64">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F64">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G64">
-        <v>4523</v>
+        <v>4639</v>
       </c>
       <c r="H64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I64" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -3039,28 +3045,28 @@
         <v>80</v>
       </c>
       <c r="B65">
-        <v>3.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C65">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D65">
-        <v>35900</v>
+        <v>32605</v>
       </c>
       <c r="E65">
         <v>15</v>
       </c>
       <c r="F65">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G65">
-        <v>5086</v>
+        <v>4469</v>
       </c>
       <c r="H65" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I65" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -3068,28 +3074,28 @@
         <v>81</v>
       </c>
       <c r="B66">
-        <v>2.9</v>
+        <v>4.2</v>
       </c>
       <c r="C66">
         <v>6</v>
       </c>
       <c r="D66">
-        <v>40695</v>
+        <v>32170</v>
       </c>
       <c r="E66">
         <v>15</v>
       </c>
       <c r="F66">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G66">
-        <v>4639</v>
+        <v>4616</v>
       </c>
       <c r="H66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I66" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -3097,25 +3103,25 @@
         <v>82</v>
       </c>
       <c r="B67">
-        <v>4.5999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D67">
-        <v>32605</v>
+        <v>33470</v>
       </c>
       <c r="E67">
         <v>15</v>
       </c>
       <c r="F67">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G67">
-        <v>4469</v>
+        <v>4968</v>
       </c>
       <c r="H67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I67" t="s">
         <v>22</v>
@@ -3126,25 +3132,25 @@
         <v>83</v>
       </c>
       <c r="B68">
-        <v>4.2</v>
+        <v>4.7</v>
       </c>
       <c r="C68">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D68">
-        <v>32170</v>
+        <v>33142</v>
       </c>
       <c r="E68">
         <v>15</v>
       </c>
       <c r="F68">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G68">
-        <v>4616</v>
+        <v>4203</v>
       </c>
       <c r="H68" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I68" t="s">
         <v>22</v>
@@ -3161,19 +3167,19 @@
         <v>6</v>
       </c>
       <c r="D69">
-        <v>33470</v>
+        <v>35870</v>
       </c>
       <c r="E69">
         <v>15</v>
       </c>
       <c r="F69">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G69">
-        <v>4968</v>
+        <v>4600</v>
       </c>
       <c r="H69" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I69" t="s">
         <v>22</v>
@@ -3184,25 +3190,25 @@
         <v>85</v>
       </c>
       <c r="B70">
-        <v>4.7</v>
+        <v>5.4</v>
       </c>
       <c r="C70">
         <v>8</v>
       </c>
       <c r="D70">
-        <v>33142</v>
+        <v>37475</v>
       </c>
       <c r="E70">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F70">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G70">
-        <v>4203</v>
+        <v>5671</v>
       </c>
       <c r="H70" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I70" t="s">
         <v>22</v>
@@ -3213,25 +3219,25 @@
         <v>86</v>
       </c>
       <c r="B71">
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="C71">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D71">
-        <v>35870</v>
+        <v>37200</v>
       </c>
       <c r="E71">
         <v>15</v>
       </c>
       <c r="F71">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G71">
-        <v>4600</v>
+        <v>5262</v>
       </c>
       <c r="H71" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I71" t="s">
         <v>22</v>
@@ -3242,25 +3248,25 @@
         <v>87</v>
       </c>
       <c r="B72">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="C72">
         <v>8</v>
       </c>
       <c r="D72">
-        <v>37475</v>
+        <v>37810</v>
       </c>
       <c r="E72">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F72">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G72">
-        <v>5671</v>
+        <v>5262</v>
       </c>
       <c r="H72" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I72" t="s">
         <v>22</v>
@@ -3271,28 +3277,28 @@
         <v>88</v>
       </c>
       <c r="B73">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="C73">
         <v>8</v>
       </c>
       <c r="D73">
-        <v>37200</v>
+        <v>35155</v>
       </c>
       <c r="E73">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F73">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G73">
-        <v>5262</v>
+        <v>5270</v>
       </c>
       <c r="H73" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I73" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -3300,25 +3306,25 @@
         <v>89</v>
       </c>
       <c r="B74">
-        <v>4.8</v>
+        <v>6</v>
       </c>
       <c r="C74">
         <v>8</v>
       </c>
       <c r="D74">
-        <v>37810</v>
+        <v>52920</v>
       </c>
       <c r="E74">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F74">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G74">
-        <v>5262</v>
+        <v>6400</v>
       </c>
       <c r="H74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I74" t="s">
         <v>22</v>
@@ -3329,28 +3335,28 @@
         <v>90</v>
       </c>
       <c r="B75">
-        <v>4.7</v>
+        <v>6</v>
       </c>
       <c r="C75">
         <v>8</v>
       </c>
       <c r="D75">
-        <v>35155</v>
+        <v>55110</v>
       </c>
       <c r="E75">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F75">
         <v>17</v>
       </c>
       <c r="G75">
-        <v>5270</v>
+        <v>5571</v>
       </c>
       <c r="H75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I75" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3358,28 +3364,28 @@
         <v>91</v>
       </c>
       <c r="B76">
-        <v>6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C76">
         <v>8</v>
       </c>
       <c r="D76">
-        <v>52920</v>
+        <v>72285</v>
       </c>
       <c r="E76">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F76">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G76">
-        <v>6400</v>
+        <v>5379</v>
       </c>
       <c r="H76" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I76" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -3387,25 +3393,25 @@
         <v>92</v>
       </c>
       <c r="B77">
-        <v>6</v>
+        <v>5.4</v>
       </c>
       <c r="C77">
         <v>8</v>
       </c>
       <c r="D77">
-        <v>55110</v>
+        <v>56140</v>
       </c>
       <c r="E77">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F77">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G77">
-        <v>5571</v>
+        <v>6041</v>
       </c>
       <c r="H77" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I77" t="s">
         <v>22</v>
@@ -3416,28 +3422,28 @@
         <v>93</v>
       </c>
       <c r="B78">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
       <c r="C78">
         <v>8</v>
       </c>
       <c r="D78">
-        <v>72285</v>
+        <v>76900</v>
       </c>
       <c r="E78">
         <v>12</v>
       </c>
       <c r="F78">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G78">
-        <v>5379</v>
+        <v>5423</v>
       </c>
       <c r="H78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I78" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -3445,28 +3451,28 @@
         <v>94</v>
       </c>
       <c r="B79">
-        <v>5.4</v>
+        <v>2.4</v>
       </c>
       <c r="C79">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D79">
-        <v>56140</v>
+        <v>19700</v>
       </c>
       <c r="E79">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F79">
+        <v>26</v>
+      </c>
+      <c r="G79">
+        <v>3441</v>
+      </c>
+      <c r="H79" t="s">
+        <v>75</v>
+      </c>
+      <c r="I79" t="s">
         <v>12</v>
-      </c>
-      <c r="G79">
-        <v>6041</v>
-      </c>
-      <c r="H79" t="s">
-        <v>77</v>
-      </c>
-      <c r="I79" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -3474,28 +3480,28 @@
         <v>95</v>
       </c>
       <c r="B80">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C80">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D80">
-        <v>76900</v>
+        <v>20400</v>
       </c>
       <c r="E80">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F80">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G80">
-        <v>5423</v>
+        <v>3181</v>
       </c>
       <c r="H80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I80" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3509,22 +3515,22 @@
         <v>4</v>
       </c>
       <c r="D81">
-        <v>19700</v>
+        <v>18380</v>
       </c>
       <c r="E81">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F81">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G81">
-        <v>3441</v>
+        <v>3648</v>
       </c>
       <c r="H81" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I81" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -3532,28 +3538,28 @@
         <v>97</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="C82">
         <v>6</v>
       </c>
       <c r="D82">
-        <v>20400</v>
+        <v>20500</v>
       </c>
       <c r="E82">
+        <v>15</v>
+      </c>
+      <c r="F82">
         <v>19</v>
       </c>
-      <c r="F82">
-        <v>25</v>
-      </c>
       <c r="G82">
-        <v>3181</v>
+        <v>3777</v>
       </c>
       <c r="H82" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I82" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -3561,85 +3567,27 @@
         <v>98</v>
       </c>
       <c r="B83">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C83">
         <v>4</v>
       </c>
       <c r="D83">
-        <v>18380</v>
+        <v>19005</v>
       </c>
       <c r="E83">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F83">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G83">
-        <v>3648</v>
+        <v>3260</v>
       </c>
       <c r="H83" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I83" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>99</v>
-      </c>
-      <c r="B84">
-        <v>3.3</v>
-      </c>
-      <c r="C84">
-        <v>6</v>
-      </c>
-      <c r="D84">
-        <v>20500</v>
-      </c>
-      <c r="E84">
-        <v>15</v>
-      </c>
-      <c r="F84">
-        <v>19</v>
-      </c>
-      <c r="G84">
-        <v>3777</v>
-      </c>
-      <c r="H84" t="s">
-        <v>77</v>
-      </c>
-      <c r="I84" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>100</v>
-      </c>
-      <c r="B85">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C85">
-        <v>4</v>
-      </c>
-      <c r="D85">
-        <v>19005</v>
-      </c>
-      <c r="E85">
-        <v>22</v>
-      </c>
-      <c r="F85">
-        <v>28</v>
-      </c>
-      <c r="G85">
-        <v>3260</v>
-      </c>
-      <c r="H85" t="s">
-        <v>77</v>
-      </c>
-      <c r="I85" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>